<commit_message>
Burndown Chart Day 9 hari ini
</commit_message>
<xml_diff>
--- a/presentasi/src/Copernicus Burn Down Chart.xlsx
+++ b/presentasi/src/Copernicus Burn Down Chart.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\presentasi\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_Presentasi_Bespoke\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="1260" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -296,6 +296,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -631,6 +699,9 @@
                 <c:pt idx="8">
                   <c:v>14</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -647,11 +718,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1501140464"/>
-        <c:axId val="1501148080"/>
+        <c:axId val="242326768"/>
+        <c:axId val="242327152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1501140464"/>
+        <c:axId val="242326768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -693,7 +764,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1501148080"/>
+        <c:crossAx val="242327152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -701,7 +772,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1501148080"/>
+        <c:axId val="242327152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -764,7 +835,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1501140464"/>
+        <c:crossAx val="242326768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1514,7 +1585,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="353637"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1774,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1911,7 +1982,9 @@
       <c r="M8" s="1">
         <v>0</v>
       </c>
-      <c r="N8" s="1"/>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -1953,7 +2026,9 @@
       <c r="M9" s="1">
         <v>0</v>
       </c>
-      <c r="N9" s="1"/>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -1995,7 +2070,9 @@
       <c r="M10" s="1">
         <v>2</v>
       </c>
-      <c r="N10" s="1"/>
+      <c r="N10" s="1">
+        <v>1</v>
+      </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -2037,7 +2114,9 @@
       <c r="M11" s="1">
         <v>3</v>
       </c>
-      <c r="N11" s="1"/>
+      <c r="N11" s="1">
+        <v>3</v>
+      </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -2079,7 +2158,9 @@
       <c r="M12" s="1">
         <v>3</v>
       </c>
-      <c r="N12" s="1"/>
+      <c r="N12" s="1">
+        <v>2</v>
+      </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -2121,7 +2202,9 @@
       <c r="M13" s="1">
         <v>6</v>
       </c>
-      <c r="N13" s="1"/>
+      <c r="N13" s="1">
+        <v>2</v>
+      </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -2213,7 +2296,10 @@
         <f>SUM(M8:M13)</f>
         <v>14</v>
       </c>
-      <c r="N15" s="1"/>
+      <c r="N15" s="1">
+        <f>SUM(N8:N13)</f>
+        <v>8</v>
+      </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>

</xml_diff>